<commit_message>
inventory, loadfile goods, delete table invent group
</commit_message>
<xml_diff>
--- a/warehouseDRF/ACCOUNTING/xls/goods — копия.xlsx
+++ b/warehouseDRF/ACCOUNTING/xls/goods — копия.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t xml:space="preserve">название</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t xml:space="preserve">книга</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пираты2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">тетрадь</t>
+  </si>
+  <si>
+    <t xml:space="preserve">пираты3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">карандаш</t>
   </si>
 </sst>
 </file>
@@ -282,10 +294,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -329,7 +341,23 @@
       <c r="C3" s="3"/>
       <c r="D3" s="1"/>
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>